<commit_message>
ALL FIGURES ARE UPDATED
</commit_message>
<xml_diff>
--- a/FILES/data/DeepBoostResult.xlsx
+++ b/FILES/data/DeepBoostResult.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9255" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9255" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="NO USE-training" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="test noise 5" sheetId="6" r:id="rId6"/>
     <sheet name="noise 10" sheetId="7" r:id="rId7"/>
     <sheet name="test noise 10" sheetId="8" r:id="rId8"/>
+    <sheet name="noise 20" sheetId="9" r:id="rId9"/>
+    <sheet name="test noise 20" sheetId="10" r:id="rId10"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -110,7 +113,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -771,7 +773,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3152,6 +3153,692 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F1" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.157142857142857</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.157142857142857</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.157142857142857</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.114285714285714</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.128571428571429</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.234421364985163</v>
+      </c>
+      <c r="C1" s="1">
+        <v>0.185714285714286</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.234421364985163</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.185714285714286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.192878338278932</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.20178041543026701</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.185714285714286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.18397626112759599</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.17142857142857101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.18991097922848699</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.185714285714286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.17507418397626101</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.185714285714286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.186943620178042</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.17142857142857101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.178041543026706</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.18100890207715101</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.17142857142857101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.172106824925816</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.18397626112759599</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.16913946587537099</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.17142857142857101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0.16320474777448099</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.166172106824926</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.172106824925816</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.166172106824926</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.166172106824926</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0.16320474777448099</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.157142857142857</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.16320474777448099</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.16023738872403601</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.15727002967358999</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.14285714285714299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0.14243323442136499</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.128571428571429</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.114285714285714</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
@@ -3310,7 +3997,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3453,7 +4140,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3586,7 +4273,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3719,7 +4406,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3851,7 +4538,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3983,8 +4670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4110,4 +4797,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D1" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E1" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F1" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.14243323442136499</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.15430267062314501</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.13946587537092001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.13946587537092001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.13946587537092001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.16320474777448099</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1513353115727</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.1513353115727</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.14540059347181</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.14836795252225499</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.14540059347181</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.14540059347181</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>